<commit_message>
Férias, verbas abertas e outros
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorago\Documents\GitHub\Orcamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorg\OneDrive\Orçamento\Sistema\DotNet\Orcamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$59</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="67">
   <si>
     <t>Colocar nome Orion no sistema.</t>
   </si>
@@ -216,16 +216,25 @@
     <t>Verificar cálculos do associados afastados</t>
   </si>
   <si>
-    <t>Desabilitar campos dos meses em que o associado não está no CR corrente</t>
-  </si>
-  <si>
     <t>Adequar os cálculos</t>
+  </si>
+  <si>
+    <t>Colocar ellipsis nos campos.</t>
+  </si>
+  <si>
+    <t>Mostrar info em pop-up das transferências enviadas.</t>
+  </si>
+  <si>
+    <t>Calcular contratações.</t>
+  </si>
+  <si>
+    <t>Mostrar férias com valor negativo em Verbas gerais no relatório resumo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -618,11 +627,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +717,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A58" si="0">A3+1</f>
+        <f t="shared" ref="A4:A61" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -990,7 +999,12 @@
       <c r="E17" s="1">
         <v>42982</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -1167,10 +1181,10 @@
         <v>42982</v>
       </c>
       <c r="F26" s="3">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1247,7 +1261,12 @@
       <c r="E30" s="1">
         <v>42982</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="3">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -1266,7 +1285,12 @@
       <c r="E31" s="1">
         <v>42982</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
@@ -1323,7 +1347,12 @@
       <c r="E34" s="1">
         <v>42982</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -1389,7 +1418,7 @@
         <v>0.5</v>
       </c>
       <c r="G37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1409,7 +1438,12 @@
       <c r="E38" s="1">
         <v>42982</v>
       </c>
-      <c r="F38" s="4"/>
+      <c r="F38" s="3">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -1663,7 +1697,7 @@
         <v>42982</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1681,8 +1715,62 @@
         <v>42989</v>
       </c>
     </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>66</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="4">
+        <v>42982</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G56">
+  <autoFilter ref="A1:G59">
     <filterColumn colId="4">
       <filters>
         <dateGroupItem year="2017" month="9" day="4" dateTimeGrouping="day"/>

</xml_diff>

<commit_message>
Trabalhando ainda no orçamento de pessoas, agora em contratações.
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="73">
   <si>
     <t>Colocar nome Orion no sistema.</t>
   </si>
@@ -216,9 +216,6 @@
     <t>Verificar cálculos do associados afastados</t>
   </si>
   <si>
-    <t>Adequar os cálculos</t>
-  </si>
-  <si>
     <t>Colocar ellipsis nos campos.</t>
   </si>
   <si>
@@ -229,6 +226,27 @@
   </si>
   <si>
     <t>Mostrar férias com valor negativo em Verbas gerais no relatório resumo</t>
+  </si>
+  <si>
+    <t>Escolher plano de convênio médico para Contratacao</t>
+  </si>
+  <si>
+    <t>Setar se contratações receberão periculosidade.</t>
+  </si>
+  <si>
+    <t>Orçar Aux. Creche para as novas contratações</t>
+  </si>
+  <si>
+    <t>Setar se pessoa contratada receberá aux. Condutor.</t>
+  </si>
+  <si>
+    <t>Verificar campos dos CRs</t>
+  </si>
+  <si>
+    <t>Adicionar diárias de viagem para pessoal da base e contratações</t>
+  </si>
+  <si>
+    <t>Valor de Previdência privada para contratações</t>
   </si>
 </sst>
 </file>
@@ -627,11 +645,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +735,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A61" si="0">A3+1</f>
+        <f t="shared" ref="A4:A68" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1184,7 +1202,7 @@
         <v>0.95</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -1415,10 +1433,10 @@
         <v>42982</v>
       </c>
       <c r="F37" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1721,7 +1739,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
@@ -1739,7 +1757,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" t="s">
         <v>38</v>
@@ -1757,15 +1775,141 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
         <v>66</v>
       </c>
-      <c r="C61" t="s">
-        <v>38</v>
-      </c>
-      <c r="D61" t="s">
-        <v>38</v>
-      </c>
-      <c r="E61" s="4">
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="4">
         <v>42982</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementando opção de salvar das premissas
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorg\OneDrive\Orçamento\Sistema\DotNet\Orcamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igorago\Documents\GitHub\Orcamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$G$68</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
   <si>
     <t>Colocar nome Orion no sistema.</t>
   </si>
@@ -247,12 +247,21 @@
   </si>
   <si>
     <t>Resumo de contratações e pessoal da base por evento (falta resumir por conta)</t>
+  </si>
+  <si>
+    <t>Corrigir menu, quando está em Orçamento, o item não fica cinza.</t>
+  </si>
+  <si>
+    <t>Corrigir menu, slide dows Premissas quando entrar no módulo</t>
+  </si>
+  <si>
+    <t>Impedir data de desligamento inferior à data de admissão ou recebimento de transferência e para funcionários transferidos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,11 +654,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +744,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A68" si="0">A3+1</f>
+        <f t="shared" ref="A4:A71" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1917,6 +1926,60 @@
       </c>
       <c r="E68" s="1">
         <v>42989</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="4">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" s="1">
+        <v>42998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>